<commit_message>
BTC and ETH are modified to BTC-USD and ETH-USD in all Resource files to fit API requirements
</commit_message>
<xml_diff>
--- a/Boris/Project_docs/Project_prototype.xlsx
+++ b/Boris/Project_docs/Project_prototype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8a693ecc95ea58f/Documents/Studies/ColumbiaBootCamp/FinTech-Workspace/Projects/Project_1_Investment_Advice/Project_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8a693ecc95ea58f/Documents/Studies/ColumbiaBootCamp/FinTech-Workspace/Projects/Project_1_Investment_Advice/FinTech_Project_1_Investment_Advice/Boris/Project_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="720" documentId="8_{D141304C-5345-49D4-A80E-12BFEDDE51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7D75A9D-BBFD-4978-9806-D3BADA1259CC}"/>
+  <xr:revisionPtr revIDLastSave="722" documentId="8_{D141304C-5345-49D4-A80E-12BFEDDE51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F811120-C2C0-4A5D-91F2-F6581080493D}"/>
   <bookViews>
-    <workbookView xWindow="-8918" yWindow="8002" windowWidth="20715" windowHeight="13276" tabRatio="775" activeTab="6" xr2:uid="{A7951F74-5094-4249-AE38-B9EBEFCE5FC0}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" tabRatio="775" activeTab="5" xr2:uid="{A7951F74-5094-4249-AE38-B9EBEFCE5FC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info to present" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="134">
   <si>
     <t>What is your current age in years?</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>Digital Assets</t>
+  </si>
+  <si>
+    <t>BTC-USD</t>
+  </si>
+  <si>
+    <t>ETH-USD</t>
   </si>
 </sst>
 </file>
@@ -833,10 +839,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2788,18 +2790,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E896DC7-392A-40EE-9E68-41806EA29EEA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
         <v>45</v>
@@ -2837,7 +2839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279BF4B4-B29D-4029-A603-462B1B37877D}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
static_data step added to the my_app.py and to the questionary_st function, my_app updated with Prrtfolio breakdowns
</commit_message>
<xml_diff>
--- a/Boris/Project_docs/Project_prototype.xlsx
+++ b/Boris/Project_docs/Project_prototype.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8a693ecc95ea58f/Documents/Studies/ColumbiaBootCamp/FinTech-Workspace/Projects/Project_1_Investment_Advice/FinTech_Project_1_Investment_Advice/Boris/Project_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="722" documentId="8_{D141304C-5345-49D4-A80E-12BFEDDE51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F811120-C2C0-4A5D-91F2-F6581080493D}"/>
+  <xr:revisionPtr revIDLastSave="733" documentId="8_{D141304C-5345-49D4-A80E-12BFEDDE51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEE19940-A343-4064-A183-70CE08EDDBCD}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" tabRatio="775" activeTab="5" xr2:uid="{A7951F74-5094-4249-AE38-B9EBEFCE5FC0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" activeTab="6" xr2:uid="{A7951F74-5094-4249-AE38-B9EBEFCE5FC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info to present" sheetId="10" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -553,6 +553,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,6 +839,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1165,7 +1171,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,9 +1240,9 @@
       <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="7">
+      <c r="S2" s="20">
         <f>SUM(S3:S16)/5</f>
-        <v>7.3999999999999996E-2</v>
+        <v>0.33200000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -1302,9 +1308,11 @@
         <v>0</v>
       </c>
       <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
         <v>1</v>
       </c>
-      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4">
         <v>0</v>
@@ -1314,11 +1322,11 @@
       </c>
       <c r="O4" s="4">
         <f>C4*I4</f>
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" ref="P4:R4" si="0">D4*J4</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="0"/>
@@ -1330,7 +1338,7 @@
       </c>
       <c r="S4" s="4">
         <f>SUM(O4:R4)</f>
-        <v>0.01</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1396,19 +1404,21 @@
         <v>1</v>
       </c>
       <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
         <v>1</v>
       </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="N7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="O7" s="4">
         <f>C7*I7</f>
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" ref="P7" si="1">D7*J7</f>
@@ -1416,7 +1426,7 @@
       </c>
       <c r="Q7" s="4">
         <f t="shared" ref="Q7" si="2">E7*K7</f>
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" ref="R7" si="3">F7*L7</f>
@@ -1424,7 +1434,7 @@
       </c>
       <c r="S7" s="4">
         <f>SUM(O7:R7)</f>
-        <v>0.01</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1490,9 +1500,11 @@
         <v>2</v>
       </c>
       <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
         <v>1</v>
       </c>
-      <c r="J10" s="4"/>
       <c r="K10" s="4">
         <v>0</v>
       </c>
@@ -1504,11 +1516,11 @@
       </c>
       <c r="O10" s="4">
         <f>C10*I10</f>
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="P10" s="4">
         <f t="shared" ref="P10" si="4">D10*J10</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" ref="Q10" si="5">E10*K10</f>
@@ -1520,7 +1532,7 @@
       </c>
       <c r="S10" s="4">
         <f>SUM(O10:R10)</f>
-        <v>0.01</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1747,7 +1759,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2122,15 +2134,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E06DF9B-83F3-4359-AC1B-2EEFEE45E952}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D1" s="17" t="s">
         <v>74</v>
       </c>
@@ -2153,7 +2165,7 @@
       <c r="O1" s="16"/>
       <c r="P1" s="16"/>
     </row>
-    <row r="2" spans="1:19" ht="207.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="207.75" x14ac:dyDescent="0.25">
       <c r="D2" s="9" t="s">
         <v>44</v>
       </c>
@@ -2196,7 +2208,7 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>39</v>
       </c>
@@ -2243,7 +2255,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>58</v>
       </c>
@@ -2342,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>59</v>
       </c>
@@ -2390,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>60</v>
       </c>
@@ -2437,8 +2449,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="W7" s="19"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.4</v>
       </c>
@@ -2489,7 +2502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>63</v>
       </c>
@@ -2537,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>62</v>
       </c>
@@ -2585,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.75</v>
       </c>
@@ -2636,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>65</v>
       </c>
@@ -2684,7 +2697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2790,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E896DC7-392A-40EE-9E68-41806EA29EEA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2839,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279BF4B4-B29D-4029-A603-462B1B37877D}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added comments to my_app.py and changed some layout
</commit_message>
<xml_diff>
--- a/Boris/Project_docs/Project_prototype.xlsx
+++ b/Boris/Project_docs/Project_prototype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8a693ecc95ea58f/Documents/Studies/ColumbiaBootCamp/FinTech-Workspace/Projects/Project_1_Investment_Advice/FinTech_Project_1_Investment_Advice/Boris/Project_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="733" documentId="8_{D141304C-5345-49D4-A80E-12BFEDDE51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEE19940-A343-4064-A183-70CE08EDDBCD}"/>
+  <xr:revisionPtr revIDLastSave="741" documentId="8_{D141304C-5345-49D4-A80E-12BFEDDE51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A5EFCBA-6C16-4250-AFA2-23B12E32CB90}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" activeTab="6" xr2:uid="{A7951F74-5094-4249-AE38-B9EBEFCE5FC0}"/>
   </bookViews>
@@ -486,13 +486,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -509,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -523,38 +523,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,7 +1157,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1226,7 @@
       <c r="R2" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="20">
+      <c r="S2" s="8">
         <f>SUM(S3:S16)/5</f>
         <v>0.33200000000000002</v>
       </c>
@@ -2137,63 +2123,72 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA5" sqref="AA5"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="9"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D1" s="17" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
       <c r="K1" s="15" t="s">
         <v>76</v>
       </c>
       <c r="L1" s="15"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="1:23" ht="207.75" x14ac:dyDescent="0.25">
-      <c r="D2" s="9" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="14" t="s">
         <v>84</v>
       </c>
       <c r="N2" s="14" t="s">
@@ -2205,545 +2200,562 @@
       <c r="P2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0</v>
-      </c>
-      <c r="K4" s="12">
-        <v>0</v>
-      </c>
-      <c r="L4" s="12">
-        <v>0</v>
-      </c>
-      <c r="M4" s="12">
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
         <v>0.1</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="11">
         <v>0.3</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="11">
         <v>0.3</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="11">
         <v>0.3</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="9">
         <f>SUM(D4:R4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="M5" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="N5" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="O5" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="P5" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="S5">
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="O5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="S5" s="9">
         <f t="shared" ref="S5:S13" si="0">SUM(D5:R5)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="L6" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="M6" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="N6" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="O6" s="13">
-        <v>0</v>
-      </c>
-      <c r="P6" s="13">
-        <v>0</v>
-      </c>
-      <c r="S6">
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="K6" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="N6" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="O6" s="11">
+        <v>0</v>
+      </c>
+      <c r="P6" s="11">
+        <v>0</v>
+      </c>
+      <c r="S6" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K7" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="L7" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="M7" s="12">
-        <v>0</v>
-      </c>
-      <c r="N7" s="13">
-        <v>0</v>
-      </c>
-      <c r="O7" s="13">
-        <v>0</v>
-      </c>
-      <c r="P7" s="13">
-        <v>0</v>
-      </c>
-      <c r="S7">
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0</v>
+      </c>
+      <c r="S7" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="W7" s="19"/>
+      <c r="W7" s="12"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="A8" s="13"/>
+      <c r="B8" s="11">
         <v>0.4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="11">
         <v>0.3</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="11">
         <v>0.3</v>
       </c>
-      <c r="J8" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K8" s="12">
-        <v>0</v>
-      </c>
-      <c r="L8" s="12">
-        <v>0</v>
-      </c>
-      <c r="M8" s="12">
-        <v>0</v>
-      </c>
-      <c r="N8" s="13">
-        <v>0</v>
-      </c>
-      <c r="O8" s="13">
-        <v>0</v>
-      </c>
-      <c r="P8" s="13">
-        <v>0</v>
-      </c>
-      <c r="S8">
+      <c r="J8" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0</v>
+      </c>
+      <c r="S8" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="J9" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K9" s="12">
-        <v>0</v>
-      </c>
-      <c r="L9" s="12">
-        <v>0</v>
-      </c>
-      <c r="M9" s="12">
-        <v>0</v>
-      </c>
-      <c r="N9" s="13">
-        <v>0</v>
-      </c>
-      <c r="O9" s="13">
-        <v>0</v>
-      </c>
-      <c r="P9" s="13">
-        <v>0</v>
-      </c>
-      <c r="S9">
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="11">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0</v>
+      </c>
+      <c r="O9" s="11">
+        <v>0</v>
+      </c>
+      <c r="P9" s="11">
+        <v>0</v>
+      </c>
+      <c r="S9" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="J10" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="K10" s="12">
-        <v>0</v>
-      </c>
-      <c r="L10" s="12">
-        <v>0</v>
-      </c>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="13">
-        <v>0</v>
-      </c>
-      <c r="O10" s="13">
-        <v>0</v>
-      </c>
-      <c r="P10" s="13">
-        <v>0</v>
-      </c>
-      <c r="S10">
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="11">
+        <v>0</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="11">
+        <v>0</v>
+      </c>
+      <c r="P10" s="11">
+        <v>0</v>
+      </c>
+      <c r="S10" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="A11" s="13"/>
+      <c r="B11" s="11">
         <v>0.75</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="11">
         <v>0.1</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="11">
         <v>0.1</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="11">
         <v>0.3</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="11">
         <v>0.3</v>
       </c>
-      <c r="H11" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0</v>
-      </c>
-      <c r="M11" s="12">
-        <v>0</v>
-      </c>
-      <c r="N11" s="13">
-        <v>0</v>
-      </c>
-      <c r="O11" s="13">
-        <v>0</v>
-      </c>
-      <c r="P11" s="13">
-        <v>0</v>
-      </c>
-      <c r="S11">
+      <c r="H11" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="11">
+        <v>0</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="11">
+        <v>0</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="I12" s="7">
-        <v>0</v>
-      </c>
-      <c r="J12" s="7">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="13">
-        <v>0</v>
-      </c>
-      <c r="O12" s="13">
-        <v>0</v>
-      </c>
-      <c r="P12" s="13">
-        <v>0</v>
-      </c>
-      <c r="S12">
+      <c r="D12" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0</v>
+      </c>
+      <c r="M12" s="11">
+        <v>0</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0</v>
+      </c>
+      <c r="S12" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="11">
         <v>0.3</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="11">
         <v>0.3</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="11">
         <v>0.3</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="11">
         <v>0.1</v>
       </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-      <c r="I13" s="7">
-        <v>0</v>
-      </c>
-      <c r="J13" s="7">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="12">
-        <v>0</v>
-      </c>
-      <c r="M13" s="12">
-        <v>0</v>
-      </c>
-      <c r="N13" s="13">
-        <v>0</v>
-      </c>
-      <c r="O13" s="13">
-        <v>0</v>
-      </c>
-      <c r="P13" s="13">
-        <v>0</v>
-      </c>
-      <c r="S13">
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
+      <c r="O13" s="11">
+        <v>0</v>
+      </c>
+      <c r="P13" s="11">
+        <v>0</v>
+      </c>
+      <c r="S13" s="9">
         <f t="shared" si="0"/>
         <v>0.99999999999999989</v>
       </c>
@@ -2765,16 +2777,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="174.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2853,7 +2865,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,308 +2878,308 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="16" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="16" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="16" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="16" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="16" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="16" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>